<commit_message>
Summary Bug fixes, completed ScoreScaleCreator chord creation Actions:
Problems
</commit_message>
<xml_diff>
--- a/src/main/resources/data/music/chordFormulas.xlsx
+++ b/src/main/resources/data/music/chordFormulas.xlsx
@@ -765,9 +765,6 @@
     <t>Six-nine</t>
   </si>
   <si>
-    <t>[6+9]</t>
-  </si>
-  <si>
     <t>[4, 3, 2, 5]</t>
   </si>
   <si>
@@ -880,6 +877,9 @@
   </si>
   <si>
     <t>C D E G</t>
+  </si>
+  <si>
+    <t>[6add9]</t>
   </si>
 </sst>
 </file>
@@ -1699,8 +1699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3171,16 +3171,16 @@
         <v>247</v>
       </c>
       <c r="B51" t="s">
-        <v>248</v>
+        <v>286</v>
       </c>
       <c r="C51" t="s">
         <v>36</v>
       </c>
       <c r="D51" t="s">
+        <v>248</v>
+      </c>
+      <c r="E51" t="s">
         <v>249</v>
-      </c>
-      <c r="E51" t="s">
-        <v>250</v>
       </c>
       <c r="F51">
         <v>4</v>
@@ -3192,24 +3192,24 @@
         <v>661</v>
       </c>
       <c r="I51" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>251</v>
+      </c>
+      <c r="B52" t="s">
         <v>252</v>
-      </c>
-      <c r="B52" t="s">
-        <v>253</v>
       </c>
       <c r="C52" t="s">
         <v>11</v>
       </c>
       <c r="D52" t="s">
+        <v>253</v>
+      </c>
+      <c r="E52" t="s">
         <v>254</v>
-      </c>
-      <c r="E52" t="s">
-        <v>255</v>
       </c>
       <c r="F52">
         <v>2</v>
@@ -3221,24 +3221,24 @@
         <v>1153</v>
       </c>
       <c r="I52" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>256</v>
+      </c>
+      <c r="B53" t="s">
         <v>257</v>
-      </c>
-      <c r="B53" t="s">
-        <v>258</v>
       </c>
       <c r="C53" t="s">
         <v>11</v>
       </c>
       <c r="D53" t="s">
+        <v>258</v>
+      </c>
+      <c r="E53" t="s">
         <v>259</v>
-      </c>
-      <c r="E53" t="s">
-        <v>260</v>
       </c>
       <c r="F53">
         <v>2</v>
@@ -3250,24 +3250,24 @@
         <v>517</v>
       </c>
       <c r="I53" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>261</v>
+      </c>
+      <c r="B54" t="s">
         <v>262</v>
-      </c>
-      <c r="B54" t="s">
-        <v>263</v>
       </c>
       <c r="C54" t="s">
         <v>11</v>
       </c>
       <c r="D54" t="s">
+        <v>263</v>
+      </c>
+      <c r="E54" t="s">
         <v>264</v>
-      </c>
-      <c r="E54" t="s">
-        <v>265</v>
       </c>
       <c r="F54">
         <v>2</v>
@@ -3279,24 +3279,24 @@
         <v>161</v>
       </c>
       <c r="I54" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>266</v>
+      </c>
+      <c r="B55" t="s">
         <v>267</v>
-      </c>
-      <c r="B55" t="s">
-        <v>268</v>
       </c>
       <c r="C55" t="s">
         <v>11</v>
       </c>
       <c r="D55" t="s">
+        <v>268</v>
+      </c>
+      <c r="E55" t="s">
         <v>269</v>
-      </c>
-      <c r="E55" t="s">
-        <v>270</v>
       </c>
       <c r="F55">
         <v>2</v>
@@ -3308,24 +3308,24 @@
         <v>641</v>
       </c>
       <c r="I55" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>271</v>
+      </c>
+      <c r="B56" t="s">
         <v>272</v>
-      </c>
-      <c r="B56" t="s">
-        <v>273</v>
       </c>
       <c r="C56" t="s">
         <v>11</v>
       </c>
       <c r="D56" t="s">
+        <v>273</v>
+      </c>
+      <c r="E56" t="s">
         <v>274</v>
-      </c>
-      <c r="E56" t="s">
-        <v>275</v>
       </c>
       <c r="F56">
         <v>2</v>
@@ -3337,24 +3337,24 @@
         <v>2177</v>
       </c>
       <c r="I56" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>276</v>
+      </c>
+      <c r="B57" t="s">
         <v>277</v>
-      </c>
-      <c r="B57" t="s">
-        <v>278</v>
       </c>
       <c r="C57" t="s">
         <v>36</v>
       </c>
       <c r="D57" t="s">
+        <v>278</v>
+      </c>
+      <c r="E57" t="s">
         <v>279</v>
-      </c>
-      <c r="E57" t="s">
-        <v>280</v>
       </c>
       <c r="F57">
         <v>3</v>
@@ -3366,24 +3366,24 @@
         <v>149</v>
       </c>
       <c r="I57" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>281</v>
+      </c>
+      <c r="B58" t="s">
         <v>282</v>
-      </c>
-      <c r="B58" t="s">
-        <v>283</v>
       </c>
       <c r="C58" t="s">
         <v>36</v>
       </c>
       <c r="D58" t="s">
+        <v>283</v>
+      </c>
+      <c r="E58" t="s">
         <v>284</v>
-      </c>
-      <c r="E58" t="s">
-        <v>285</v>
       </c>
       <c r="F58">
         <v>3</v>
@@ -3395,7 +3395,7 @@
         <v>149</v>
       </c>
       <c r="I58" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>